<commit_message>
Revised fix to not kill SQL (good data)
</commit_message>
<xml_diff>
--- a/benchmark_results.xlsx
+++ b/benchmark_results.xlsx
@@ -218,7 +218,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -268,31 +270,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.075</c:v>
+                  <c:v>1.089</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.049</c:v>
+                  <c:v>0.047</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.868</c:v>
+                  <c:v>1.862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.199</c:v>
+                  <c:v>0.201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45</c:v>
+                  <c:v>0.458</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.258</c:v>
+                  <c:v>34.943</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.06</c:v>
+                  <c:v>0.057</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.056</c:v>
+                  <c:v>0.064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -308,6 +310,104 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Mongo (2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>testShortestPathBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>testFindWithFilterBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>testCountPublicationsForYearIntervalBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>testCountAllPublicationsForConferenceBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>testFindOrderedByBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>testAverageAuthorsForPublicationBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>testFindPublicationById</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>testCountAllAuthorsForConferenceBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>testCoauthorsBenchmark</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.047</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.447</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.787</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.059</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.058</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Db4o(1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -359,58 +459,58 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.175</c:v>
+                  <c:v>2.355</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.089</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.381</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.909</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.006</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.049</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.839</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.205</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.47</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30.262</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.056</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.057</c:v>
+                  <c:v>1.844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Db4o(1)</c:v>
+                  <c:v>Db4o(2)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -455,132 +555,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4.187</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.395</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>31.44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.251</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.351</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45.657</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.008</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.045</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.581</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Db4o(2)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>testShortestPathBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>testFindWithFilterBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>testCountPublicationsForYearIntervalBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>testCountAllPublicationsForConferenceBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>testFindOrderedByBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>testAverageAuthorsForPublicationBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>testFindPublicationById</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>testCountAllAuthorsForConferenceBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>testCoauthorsBenchmark</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet1!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.224</c:v>
+                  <c:v>2.414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.329</c:v>
+                  <c:v>1.504</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.725</c:v>
+                  <c:v>31.511</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.236</c:v>
+                  <c:v>0.089</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.425</c:v>
+                  <c:v>4.365</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44.738</c:v>
+                  <c:v>20.082</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.01</c:v>
+                  <c:v>0.005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.043</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.384</c:v>
+                  <c:v>1.771</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -602,10 +606,12 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -651,6 +657,33 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.292</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.561</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.405</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.069</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.714</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.927</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.069</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.854</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -720,6 +753,33 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.562</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.954</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.794</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.021</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.046</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.031</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1765,7 +1825,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1801,16 +1861,22 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1.075</v>
+        <v>1.089</v>
       </c>
       <c r="C2">
-        <v>1.175</v>
+        <v>1.101</v>
       </c>
       <c r="D2">
-        <v>4.1870000000000003</v>
+        <v>2.355</v>
       </c>
       <c r="E2">
-        <v>4.2240000000000002</v>
+        <v>2.4140000000000001</v>
+      </c>
+      <c r="F2">
+        <v>2.2919999999999998</v>
+      </c>
+      <c r="G2">
+        <v>1.931</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1818,16 +1884,22 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>4.9000000000000002E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="C3">
-        <v>4.9000000000000002E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="D3">
-        <v>4.3949999999999996</v>
+        <v>1.5089999999999999</v>
       </c>
       <c r="E3">
-        <v>4.3289999999999997</v>
+        <v>1.504</v>
+      </c>
+      <c r="F3">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="G3">
+        <v>0.56200000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1835,16 +1907,22 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1.8680000000000001</v>
+        <v>1.8620000000000001</v>
       </c>
       <c r="C4">
-        <v>1.839</v>
+        <v>1.9279999999999999</v>
       </c>
       <c r="D4">
-        <v>31.44</v>
+        <v>31.01</v>
       </c>
       <c r="E4">
-        <v>32.725000000000001</v>
+        <v>31.510999999999999</v>
+      </c>
+      <c r="F4">
+        <v>7.4050000000000002</v>
+      </c>
+      <c r="G4">
+        <v>6.9539999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1852,16 +1930,22 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.19900000000000001</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="C5">
         <v>0.20499999999999999</v>
       </c>
       <c r="D5">
-        <v>0.251</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E5">
-        <v>0.23599999999999999</v>
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="F5">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G5">
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1869,16 +1953,22 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.45</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="C6">
-        <v>0.47</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="D6">
-        <v>4.351</v>
+        <v>4.3810000000000002</v>
       </c>
       <c r="E6">
-        <v>4.4249999999999998</v>
+        <v>4.3650000000000002</v>
+      </c>
+      <c r="F6">
+        <v>0.71</v>
+      </c>
+      <c r="G6">
+        <v>0.79400000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1886,16 +1976,22 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>31.257999999999999</v>
+        <v>34.942999999999998</v>
       </c>
       <c r="C7">
-        <v>30.262</v>
+        <v>35.786999999999999</v>
       </c>
       <c r="D7">
-        <v>45.656999999999996</v>
+        <v>18.908999999999999</v>
       </c>
       <c r="E7">
-        <v>44.738</v>
+        <v>20.082000000000001</v>
+      </c>
+      <c r="F7">
+        <v>36.713999999999999</v>
+      </c>
+      <c r="G7">
+        <v>36.1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1906,13 +2002,19 @@
         <v>1E-3</v>
       </c>
       <c r="C8">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D8">
-        <v>8.0000000000000002E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E8">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>1.927</v>
+      </c>
+      <c r="G8">
+        <v>2.0209999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1920,16 +2022,22 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.06</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="C9">
-        <v>5.6000000000000001E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D9">
-        <v>4.4999999999999998E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E9">
-        <v>4.2999999999999997E-2</v>
+        <v>0.03</v>
+      </c>
+      <c r="F9">
+        <v>1.069</v>
+      </c>
+      <c r="G9">
+        <v>1.046</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1937,16 +2045,22 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>5.6000000000000001E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="C10">
-        <v>5.7000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D10">
-        <v>1.581</v>
+        <v>1.8440000000000001</v>
       </c>
       <c r="E10">
-        <v>1.3839999999999999</v>
+        <v>1.7709999999999999</v>
+      </c>
+      <c r="F10">
+        <v>1.8540000000000001</v>
+      </c>
+      <c r="G10">
+        <v>2.0310000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>